<commit_message>
renamed variables for use in attribute mapper
renamed date variables, description, organization title
</commit_message>
<xml_diff>
--- a/docs/NB_AttributeSource_V1.xlsx
+++ b/docs/NB_AttributeSource_V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/NRCAN/fgp-metadata-proxy/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0746F9D-5278-DB4A-9969-3BDB8B423744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1787352-5EF9-4343-AF96-35F0A6B98038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21600" yWindow="6660" windowWidth="21600" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E9"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1197,19 +1197,19 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1571,19 +1571,19 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="7" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started implementing selenium python package installation instructions
</commit_message>
<xml_diff>
--- a/docs/NB_AttributeSource_V1.xlsx
+++ b/docs/NB_AttributeSource_V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/NRCAN/fgp-metadata-proxy/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1787352-5EF9-4343-AF96-35F0A6B98038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C036F5BB-1025-604C-A782-05805DC55D97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21600" yWindow="6660" windowWidth="21600" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:E32"/>
+    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2013,19 +2013,19 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="A58" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="7" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Default_NB lookup table
Added default_NB lookup table
</commit_message>
<xml_diff>
--- a/docs/NB_AttributeSource_V1.xlsx
+++ b/docs/NB_AttributeSource_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/NRCAN/fgp-metadata-proxy/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C036F5BB-1025-604C-A782-05805DC55D97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F35723-D72D-3B41-BB9E-F337C55BE4B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="6660" windowWidth="21600" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="6660" windowWidth="21600" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -697,7 +697,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -707,6 +707,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,11 +735,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -747,7 +756,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,16 +1061,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="B69" sqref="A69:XFD70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="57.5" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="64.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="64.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="43" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1050,10 +1081,10 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E1" t="s">
@@ -1061,70 +1092,70 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1135,81 +1166,81 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>150</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1220,47 +1251,47 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>156</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="E12" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="6" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1271,30 +1302,30 @@
       <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1305,81 +1336,81 @@
       <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" s="6" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="E17" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="E18" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="E19" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C20" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1390,10 +1421,10 @@
       <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E21" t="s">
@@ -1407,10 +1438,10 @@
       <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>164</v>
       </c>
       <c r="E22" t="s">
@@ -1424,30 +1455,30 @@
       <c r="B23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1458,10 +1489,10 @@
       <c r="B25" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>166</v>
       </c>
       <c r="E25" t="s">
@@ -1469,155 +1500,155 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="E29" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="C30" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="E30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="E30" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="C31" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="E32" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="C33" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="E33" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="E33" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="C34" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1628,64 +1659,64 @@
       <c r="B35" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>172</v>
       </c>
       <c r="E35" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="C36" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="E36" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="E36" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C37" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="E37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="E37" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C38" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1696,30 +1727,30 @@
       <c r="B39" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="C39" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>177</v>
       </c>
       <c r="E39" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="C40" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1730,10 +1761,10 @@
       <c r="B41" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="C41" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>177</v>
       </c>
       <c r="E41" t="s">
@@ -1741,53 +1772,53 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D42" s="8" t="s">
+      <c r="C42" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D43" s="8" t="s">
+      <c r="C43" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="E43" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="C44" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1798,30 +1829,30 @@
       <c r="B45" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>179</v>
       </c>
       <c r="E45" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="6" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1832,10 +1863,10 @@
       <c r="B47" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>183</v>
       </c>
       <c r="E47" t="s">
@@ -1849,81 +1880,81 @@
       <c r="B48" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="1" t="s">
         <v>184</v>
       </c>
       <c r="E48" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="49" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="C49" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="50" spans="1:5" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D50" s="4" t="s">
+      <c r="C50" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="51" spans="1:5" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D51" s="4" t="s">
+      <c r="C51" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="52" spans="1:5" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D52" s="4" t="s">
+      <c r="C52" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D52" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="12" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1934,30 +1965,30 @@
       <c r="B53" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D53" s="4" t="s">
+      <c r="C53" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>186</v>
       </c>
       <c r="E53" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="54" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D54" s="4" t="s">
+      <c r="C54" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="6" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1968,30 +1999,30 @@
       <c r="B55" t="s">
         <v>93</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D55" s="4" t="s">
+      <c r="C55" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>186</v>
       </c>
       <c r="E55" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D56" s="4" t="s">
+      <c r="C56" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D56" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="6" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2002,10 +2033,10 @@
       <c r="B57" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="C57" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>189</v>
       </c>
       <c r="E57" t="s">
@@ -2013,19 +2044,19 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E58" s="6" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2036,10 +2067,10 @@
       <c r="B59" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="4" t="s">
         <v>189</v>
       </c>
       <c r="E59" t="s">
@@ -2053,10 +2084,10 @@
       <c r="B60" t="s">
         <v>104</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="1" t="s">
         <v>198</v>
       </c>
       <c r="E60" t="s">
@@ -2070,10 +2101,10 @@
       <c r="B61" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D61" s="2" t="s">
+      <c r="C61" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>196</v>
       </c>
       <c r="E61" t="s">
@@ -2087,10 +2118,10 @@
       <c r="B62" t="s">
         <v>107</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="4" t="s">
         <v>189</v>
       </c>
       <c r="E62" t="s">
@@ -2104,10 +2135,10 @@
       <c r="B63" t="s">
         <v>109</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D63" s="6" t="s">
+      <c r="C63" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>191</v>
       </c>
       <c r="E63" t="s">
@@ -2121,10 +2152,10 @@
       <c r="B64" t="s">
         <v>111</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D64" s="1" t="s">
         <v>198</v>
       </c>
       <c r="E64" t="s">
@@ -2138,10 +2169,10 @@
       <c r="B65" t="s">
         <v>113</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="4" t="s">
         <v>189</v>
       </c>
       <c r="E65" t="s">
@@ -2155,30 +2186,30 @@
       <c r="B66" t="s">
         <v>115</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D66" s="6" t="s">
+      <c r="C66" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>191</v>
       </c>
       <c r="E66" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="67" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D67" s="5" t="s">
+      <c r="C67" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D67" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="6" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2189,217 +2220,217 @@
       <c r="B68" t="s">
         <v>119</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D68" s="5" t="s">
+      <c r="C68" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>189</v>
       </c>
       <c r="E68" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="69" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D69" s="2" t="s">
+      <c r="C69" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="E69" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="E69" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D70" s="4" t="s">
+      <c r="C70" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="E70" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="E70" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D71" s="2" t="s">
+      <c r="C71" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D71" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="E71" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="E71" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D72" s="1" t="s">
+      <c r="C72" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E72" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="E72" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A73" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D73" s="2" t="s">
+      <c r="C73" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D73" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C74" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D74" s="8" t="s">
+      <c r="C74" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D74" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="E74" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B75" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C75" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D75" s="8" t="s">
+      <c r="C75" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D75" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E75" s="7" t="s">
+      <c r="E75" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C76" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D76" s="8" t="s">
+      <c r="C76" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D76" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E76" s="7" t="s">
+      <c r="E76" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C77" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D77" s="8" t="s">
+      <c r="C77" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E77" s="7" t="s">
+      <c r="E77" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C78" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D78" s="8" t="s">
+      <c r="C78" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D78" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E78" s="7" t="s">
+      <c r="E78" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B79" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C79" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D79" s="8" t="s">
+      <c r="C79" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D79" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E79" s="7" t="s">
+      <c r="E79" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C80" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D80" s="8" t="s">
+      <c r="C80" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D80" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E80" s="7" t="s">
+      <c r="E80" s="6" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
french tags to remove
added french tags to remove lookup table
</commit_message>
<xml_diff>
--- a/docs/NB_AttributeSource_V1.xlsx
+++ b/docs/NB_AttributeSource_V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/NRCAN/fgp-metadata-proxy/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5BC57F-802B-404B-B339-463032F37CC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15202242-0554-FF42-BBE5-CA2EAC0B230E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28620" yWindow="12640" windowWidth="21600" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1061,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1482,20 +1482,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="C25" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2077,20 +2077,20 @@
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="60" spans="1:5" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="6" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2145,20 +2145,20 @@
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="64" spans="1:5" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="6" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added wgs84 EPSG codes for default socrata datasets
</commit_message>
<xml_diff>
--- a/docs/NB_AttributeSource_V1.xlsx
+++ b/docs/NB_AttributeSource_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/NRCAN/fgp-metadata-proxy/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15202242-0554-FF42-BBE5-CA2EAC0B230E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84C010D-2432-5C4A-8522-5703DEAF75D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28620" yWindow="12640" windowWidth="21600" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28620" yWindow="12700" windowWidth="21600" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1061,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1856,20 +1856,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:5" s="6" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="6" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to lookup tables
</commit_message>
<xml_diff>
--- a/docs/NB_AttributeSource_V1.xlsx
+++ b/docs/NB_AttributeSource_V1.xlsx
@@ -8,17 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/NRCAN/fgp-metadata-proxy/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84C010D-2432-5C4A-8522-5703DEAF75D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABA0639-247D-EA4A-AB33-7366804801ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28620" yWindow="12700" windowWidth="21600" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36940" yWindow="13280" windowWidth="21600" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -697,7 +705,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -716,12 +724,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -735,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -759,24 +761,17 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1061,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1322,7 +1317,7 @@
       <c r="C15" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="10" t="s">
         <v>158</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -1849,7 +1844,7 @@
       <c r="C46" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="11" t="s">
         <v>181</v>
       </c>
       <c r="E46" s="6" t="s">
@@ -1917,7 +1912,7 @@
       <c r="C50" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" s="9" t="s">
         <v>185</v>
       </c>
       <c r="E50" s="12" t="s">
@@ -1934,7 +1929,7 @@
       <c r="C51" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="9" t="s">
         <v>185</v>
       </c>
       <c r="E51" s="12" t="s">
@@ -1951,7 +1946,7 @@
       <c r="C52" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="9" t="s">
         <v>185</v>
       </c>
       <c r="E52" s="12" t="s">
@@ -1985,7 +1980,7 @@
       <c r="C54" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="10" t="s">
         <v>185</v>
       </c>
       <c r="E54" s="6" t="s">
@@ -2019,7 +2014,7 @@
       <c r="C56" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="10" t="s">
         <v>188</v>
       </c>
       <c r="E56" s="6" t="s">
@@ -2206,7 +2201,7 @@
       <c r="C67" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="11" t="s">
         <v>151</v>
       </c>
       <c r="E67" s="6" t="s">
@@ -2257,61 +2252,61 @@
       <c r="C70" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D70" s="15" t="s">
+      <c r="D70" s="10" t="s">
         <v>192</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A71" s="9" t="s">
+    <row r="71" spans="1:5" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A71" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C71" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D71" s="10" t="s">
+      <c r="C71" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D71" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E71" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
+      <c r="E71" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C72" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D72" s="11" t="s">
+      <c r="C72" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E72" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A73" s="9" t="s">
+      <c r="E72" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A73" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C73" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D73" s="10" t="s">
+      <c r="C73" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D73" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E73" s="9" t="s">
+      <c r="E73" s="6" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Metadata Value Mapping and Format Mapping
</commit_message>
<xml_diff>
--- a/docs/NB_AttributeSource_V1.xlsx
+++ b/docs/NB_AttributeSource_V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/NRCAN/fgp-metadata-proxy/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABA0639-247D-EA4A-AB33-7366804801ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE24484-1464-2444-ADA5-CEF28659B476}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36940" yWindow="13280" windowWidth="21600" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -745,13 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1056,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD52"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1087,70 +1081,70 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1171,71 +1165,71 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1256,394 +1250,394 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="E12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="E13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="E14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D15" s="10" t="s">
+      <c r="C15" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="E15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C16" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="E18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="E19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="C20" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="E20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="C21" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="E21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="E22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="C23" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="E23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D24" s="7" t="s">
+      <c r="C24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="E24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D25" s="7" t="s">
+      <c r="C25" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="E29" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D30" s="7" t="s">
+      <c r="C30" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+      <c r="E30" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" s="7" t="s">
+      <c r="C31" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="E32" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="7" t="s">
+      <c r="C33" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+      <c r="E33" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D34" s="8" t="s">
+      <c r="C34" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1664,156 +1658,156 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D36" s="7" t="s">
+      <c r="C36" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+      <c r="E36" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D37" s="7" t="s">
+      <c r="C37" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+      <c r="E37" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D38" s="8" t="s">
+      <c r="C38" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="E38" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C39" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E39" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+      <c r="E39" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D40" s="8" t="s">
+      <c r="C40" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="E40" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="C41" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D42" s="7" t="s">
+      <c r="C42" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D43" s="7" t="s">
+      <c r="C43" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+      <c r="E43" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D44" s="8" t="s">
+      <c r="C44" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1827,44 +1821,44 @@
       <c r="C45" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="3" t="s">
         <v>179</v>
       </c>
       <c r="E45" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+    <row r="46" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D46" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="6" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+    <row r="47" spans="1:5" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E47" s="4" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1885,139 +1879,139 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
+    <row r="49" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D49" s="8" t="s">
+      <c r="C49" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="E49" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="s">
+    <row r="50" spans="1:5" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="D50" s="9" t="s">
+      <c r="C50" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="12" t="s">
+    <row r="51" spans="1:5" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="D51" s="9" t="s">
+      <c r="C51" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="12" t="s">
+    <row r="52" spans="1:5" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="D52" s="9" t="s">
+      <c r="C52" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D53" s="3" t="s">
+      <c r="C53" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
+    <row r="54" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D54" s="10" t="s">
+      <c r="C54" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="E54" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="55" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D55" s="3" t="s">
+      <c r="C55" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C56" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D56" s="10" t="s">
+      <c r="C56" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="E56" s="4" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2031,7 +2025,7 @@
       <c r="C57" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="3" t="s">
         <v>189</v>
       </c>
       <c r="E57" t="s">
@@ -2039,19 +2033,19 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="4" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2065,27 +2059,27 @@
       <c r="C59" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="3" t="s">
         <v>189</v>
       </c>
       <c r="E59" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
+    <row r="60" spans="1:5" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="4" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2116,44 +2110,44 @@
       <c r="C62" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="3" t="s">
         <v>189</v>
       </c>
       <c r="E62" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="63" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D63" s="5" t="s">
+      <c r="C63" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
+    <row r="64" spans="1:5" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="E64" s="4" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2167,44 +2161,44 @@
       <c r="C65" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="3" t="s">
         <v>189</v>
       </c>
       <c r="E65" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="66" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D66" s="5" t="s">
+      <c r="C66" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
+    <row r="67" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C67" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D67" s="11" t="s">
+      <c r="C67" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D67" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="E67" s="4" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2218,214 +2212,214 @@
       <c r="C68" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="3" t="s">
         <v>189</v>
       </c>
       <c r="E68" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
+    <row r="69" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C69" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D69" s="7" t="s">
+      <c r="C69" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
+      <c r="E69" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C70" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D70" s="10" t="s">
+      <c r="C70" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="E70" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
+      <c r="E70" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C71" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D71" s="7" t="s">
+      <c r="C71" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="E71" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
+      <c r="E71" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C72" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D72" s="8" t="s">
+      <c r="C72" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E72" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
+      <c r="E72" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C73" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D73" s="7" t="s">
+      <c r="C73" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="E73" s="6" t="s">
+      <c r="E73" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C74" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D74" s="7" t="s">
+      <c r="C74" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D74" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E74" s="6" t="s">
+      <c r="E74" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D75" s="7" t="s">
+      <c r="C75" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D75" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E75" s="6" t="s">
+      <c r="E75" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
+      <c r="A76" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C76" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D76" s="7" t="s">
+      <c r="C76" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E76" s="6" t="s">
+      <c r="E76" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
+      <c r="A77" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C77" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D77" s="7" t="s">
+      <c r="C77" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D77" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E77" s="6" t="s">
+      <c r="E77" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
+      <c r="A78" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C78" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D78" s="7" t="s">
+      <c r="C78" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E78" s="6" t="s">
+      <c r="E78" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D79" s="7" t="s">
+      <c r="C79" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="E79" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C80" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D80" s="7" t="s">
+      <c r="C80" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="E80" s="4" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added AWS Translate Step
</commit_message>
<xml_diff>
--- a/docs/NB_AttributeSource_V1.xlsx
+++ b/docs/NB_AttributeSource_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/NRCAN/fgp-metadata-proxy/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE24484-1464-2444-ADA5-CEF28659B476}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2689FF9A-E806-FF48-80D5-B3B4E92375A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36940" yWindow="13280" windowWidth="21600" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36940" yWindow="13280" windowWidth="24660" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1148,20 +1148,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1233,20 +1233,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1641,20 +1641,20 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1862,20 +1862,20 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="48" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="4" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2083,20 +2083,20 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="61" spans="1:5" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D61" s="1" t="s">
+      <c r="C61" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="4" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>